<commit_message>
Updated code and README file
</commit_message>
<xml_diff>
--- a/Task_Distribution/output.xlsx
+++ b/Task_Distribution/output.xlsx
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(4)</t>
+          <t>MME235-2016-17-(2)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(11)</t>
+          <t>MME235-2014-15-(6)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(4)</t>
+          <t>EEE267-2014-15-(1)</t>
         </is>
       </c>
     </row>
@@ -481,17 +481,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(3)</t>
+          <t>ME221-2018-19-(1)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(11)</t>
+          <t>ME221-2014-15-(4)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(5)</t>
+          <t>EEE267-2017-18-(4)</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ME221-2014-15-(3)</t>
+          <t>MME213-2015-16-(8)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(8)</t>
+          <t>ME221-2015-16-(8)</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(2)</t>
+          <t>EEE267-2016-17-(3)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(7)</t>
+          <t>EEE267-2015-16-(8)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(7)</t>
+          <t>EEE267-2017-18-(8)</t>
         </is>
       </c>
     </row>
@@ -541,17 +541,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(6)</t>
+          <t>MME213-2014-15-(12)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(1)</t>
+          <t>MME213-2018-19-(4)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(5)</t>
+          <t>ME221-2015-16-(5)</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(8)</t>
+          <t>EEE267-2018-19-(2)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(2)</t>
+          <t>EEE267-2018-19-(8)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(7)</t>
+          <t>MME213-2016-17-(6)</t>
         </is>
       </c>
     </row>
@@ -581,17 +581,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(2)</t>
+          <t>ME221-2016-17-(3)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(1)</t>
+          <t>MME213-2015-16-(9)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(7)</t>
+          <t>MME213-2016-17-(9)</t>
         </is>
       </c>
     </row>
@@ -601,17 +601,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MME235-2015-16-(3)</t>
+          <t>ME221-2014-15-(7)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(5)</t>
+          <t>EEE267-2015-16-(5)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(8)</t>
+          <t>MME235-2017-18-(3)</t>
         </is>
       </c>
     </row>
@@ -621,17 +621,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(12)</t>
+          <t>MME213-2017-18-(4)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(4)</t>
+          <t>EEE267-2017-18-(1)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(5)</t>
+          <t>ME221-2015-16-(2)</t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(2)</t>
+          <t>MME235-2017-18-(6)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(4)</t>
+          <t>MME213-2018-19-(7)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(3)</t>
+          <t>MME213-2014-15-(5)</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(7)</t>
+          <t>MME235-2018-19-(6)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(7)</t>
+          <t>MME235-2015-16-(1)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(2)</t>
+          <t>MME213-2014-15-(8)</t>
         </is>
       </c>
     </row>
@@ -681,17 +681,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(8)</t>
+          <t>ME221-2017-18-(3)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(7)</t>
+          <t>MME213-2016-17-(3)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(4)</t>
+          <t>EEE267-2018-19-(1)</t>
         </is>
       </c>
     </row>
@@ -701,17 +701,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(7)</t>
+          <t>ME221-2017-18-(8)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(2)</t>
+          <t>ME221-2016-17-(1)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>MME235-2018-19-(2)</t>
+          <t>MME213-2015-16-(5)</t>
         </is>
       </c>
     </row>
@@ -721,17 +721,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(3)</t>
+          <t>ME221-2017-18-(4)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(10)</t>
+          <t>ME221-2015-16-(7)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(5)</t>
+          <t>EEE267-2014-15-(3)</t>
         </is>
       </c>
     </row>
@@ -741,17 +741,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(6)</t>
+          <t>MME235-2015-16-(2)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MME235-2015-16-(1)</t>
+          <t>MME213-2018-19-(8)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(2)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -761,17 +761,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(4)</t>
+          <t>EEE267-2014-15-(7)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(3)</t>
+          <t>MME213-2017-18-(8)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(4)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(6)</t>
+          <t>MME213-2015-16-(11)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(1)</t>
+          <t>MME213-2018-19-(6)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(8)</t>
+          <t>ME221-2018-19-(2)</t>
         </is>
       </c>
     </row>
@@ -801,17 +801,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(9)</t>
+          <t>EEE267-2014-15-(6)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(1)</t>
+          <t>MME213-2016-17-(1)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(4)</t>
+          <t>EEE267-2016-17-(4)</t>
         </is>
       </c>
     </row>
@@ -821,17 +821,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(7)</t>
+          <t>MME235-2014-15-(5)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(6)</t>
+          <t>MME213-2016-17-(5)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(1)</t>
+          <t>MME235-2017-18-(8)</t>
         </is>
       </c>
     </row>
@@ -841,17 +841,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(7)</t>
+          <t>MME213-2014-15-(3)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(3)</t>
+          <t>EEE267-2015-16-(2)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(1)</t>
+          <t>MME235-2017-18-(4)</t>
         </is>
       </c>
     </row>
@@ -861,17 +861,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(11)</t>
+          <t>MME213-2015-16-(1)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(5)</t>
+          <t>ME221-2018-19-(3)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(4)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -881,17 +881,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(8)</t>
+          <t>MME235-2016-17-(3)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(7)</t>
+          <t>MME213-2014-15-(7)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(8)</t>
+          <t>ME221-2018-19-(8)</t>
         </is>
       </c>
     </row>
@@ -901,17 +901,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(2)</t>
+          <t>EEE267-2016-17-(7)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(1)</t>
+          <t>EEE267-2016-17-(5)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(3)</t>
+          <t>ME221-2017-18-(6)</t>
         </is>
       </c>
     </row>
@@ -921,17 +921,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(5)</t>
+          <t>ME221-2018-19-(4)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(5)</t>
+          <t>ME221-2015-16-(6)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(7)</t>
+          <t>MME213-2016-17-(12)</t>
         </is>
       </c>
     </row>
@@ -941,17 +941,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(6)</t>
+          <t>EEE267-2015-16-(6)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(7)</t>
+          <t>EEE267-2014-15-(8)</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(12)</t>
+          <t>MME235-2014-15-(3)</t>
         </is>
       </c>
     </row>
@@ -961,17 +961,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MME235-2015-16-(6)</t>
+          <t>EEE267-2017-18-(7)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(11)</t>
+          <t>MME213-2016-17-(10)</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(7)</t>
+          <t>MME235-2018-19-(2)</t>
         </is>
       </c>
     </row>
@@ -981,17 +981,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(8)</t>
+          <t>ME221-2014-15-(1)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(7)</t>
+          <t>MME213-2015-16-(12)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(3)</t>
+          <t>EEE267-2017-18-(2)</t>
         </is>
       </c>
     </row>
@@ -1001,17 +1001,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ME221-2014-15-(1)</t>
+          <t>MME213-2016-17-(8)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(2)</t>
+          <t>EEE267-2018-19-(3)</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(9)</t>
+          <t>ME221-2014-15-(3)</t>
         </is>
       </c>
     </row>
@@ -1021,17 +1021,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>MME235-2015-16-(4)</t>
+          <t>MME235-2016-17-(8)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(1)</t>
+          <t>EEE267-2018-19-(4)</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(2)</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1041,17 +1041,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(1)</t>
+          <t>MME213-2018-19-(2)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(1)</t>
+          <t>MME213-2016-17-(7)</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(2)</t>
+          <t>EEE267-2015-16-(3)</t>
         </is>
       </c>
     </row>
@@ -1061,17 +1061,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(6)</t>
+          <t>ME221-2014-15-(6)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>EEE267-2014-15-(4)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>MME235-2018-19-(4)</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>-</t>
         </is>
       </c>
     </row>
@@ -1081,17 +1081,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(10)</t>
+          <t>EEE267-2017-18-(3)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(5)</t>
+          <t>MME213-2018-19-(1)</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>MME235-2018-19-(1)</t>
+          <t>MME235-2017-18-(5)</t>
         </is>
       </c>
     </row>
@@ -1101,17 +1101,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(1)</t>
+          <t>MME235-2014-15-(4)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(2)</t>
+          <t>ME221-2017-18-(5)</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MME235-2014-15-(7)</t>
         </is>
       </c>
     </row>
@@ -1121,17 +1121,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>MME235-2015-16-(6)</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>MME213-2017-18-(5)</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>ME221-2014-15-(5)</t>
-        </is>
-      </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(5)</t>
+          <t>MME213-2016-17-(11)</t>
         </is>
       </c>
     </row>
@@ -1141,17 +1141,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(10)</t>
+          <t>ME221-2017-18-(2)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(12)</t>
+          <t>MME235-2014-15-(8)</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(9)</t>
+          <t>MME235-2016-17-(7)</t>
         </is>
       </c>
     </row>
@@ -1161,17 +1161,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(5)</t>
+          <t>MME213-2017-18-(10)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(8)</t>
+          <t>ME221-2016-17-(5)</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ME221-2014-15-(7)</t>
+          <t>EEE267-2014-15-(2)</t>
         </is>
       </c>
     </row>
@@ -1181,17 +1181,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ME221-2014-15-(4)</t>
+          <t>ME221-2016-17-(2)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(2)</t>
+          <t>MME235-2014-15-(1)</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(3)</t>
+          <t>MME213-2015-16-(6)</t>
         </is>
       </c>
     </row>
@@ -1201,17 +1201,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(6)</t>
+          <t>MME213-2014-15-(10)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(2)</t>
+          <t>ME221-2017-18-(7)</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(5)</t>
+          <t>MME235-2017-18-(2)</t>
         </is>
       </c>
     </row>
@@ -1221,17 +1221,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(8)</t>
+          <t>ME221-2018-19-(7)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(8)</t>
+          <t>MME235-2014-15-(2)</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(6)</t>
+          <t>MME213-2015-16-(7)</t>
         </is>
       </c>
     </row>
@@ -1241,17 +1241,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(4)</t>
+          <t>MME235-2016-17-(5)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(5)</t>
+          <t>EEE267-2016-17-(2)</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(6)</t>
+          <t>MME213-2017-18-(3)</t>
         </is>
       </c>
     </row>
@@ -1261,17 +1261,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(4)</t>
+          <t>MME235-2015-16-(3)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(8)</t>
+          <t>MME235-2015-16-(5)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MME213-2018-19-(3)</t>
         </is>
       </c>
     </row>
@@ -1281,17 +1281,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>MME235-2015-16-(7)</t>
+          <t>MME213-2014-15-(2)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ME221-2014-15-(2)</t>
+          <t>MME213-2017-18-(7)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(12)</t>
+          <t>ME221-2014-15-(5)</t>
         </is>
       </c>
     </row>
@@ -1301,17 +1301,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(6)</t>
+          <t>EEE267-2017-18-(6)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(3)</t>
+          <t>ME221-2014-15-(2)</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(8)</t>
+          <t>ME221-2015-16-(1)</t>
         </is>
       </c>
     </row>
@@ -1321,17 +1321,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(7)</t>
+          <t>ME221-2014-15-(8)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(10)</t>
+          <t>EEE267-2015-16-(4)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(4)</t>
+          <t>MME213-2017-18-(12)</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(6)</t>
+          <t>MME213-2014-15-(1)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(3)</t>
+          <t>MME213-2015-16-(2)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>MME235-2015-16-(2)</t>
+          <t>MME213-2014-15-(6)</t>
         </is>
       </c>
     </row>
@@ -1361,17 +1361,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(5)</t>
+          <t>EEE267-2015-16-(1)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MME235-2015-16-(5)</t>
+          <t>ME221-2016-17-(7)</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>MME235-2018-19-(7)</t>
+          <t>MME235-2016-17-(4)</t>
         </is>
       </c>
     </row>
@@ -1381,17 +1381,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ME221-2017-18-(4)</t>
+          <t>ME221-2016-17-(8)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(6)</t>
+          <t>MME235-2018-19-(1)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(1)</t>
+          <t>MME235-2018-19-(3)</t>
         </is>
       </c>
     </row>
@@ -1401,17 +1401,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ME221-2015-16-(3)</t>
+          <t>MME235-2018-19-(7)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(3)</t>
+          <t>MME213-2017-18-(2)</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(5)</t>
+          <t>EEE267-2014-15-(5)</t>
         </is>
       </c>
     </row>
@@ -1421,17 +1421,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(1)</t>
+          <t>MME235-2018-19-(5)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(8)</t>
+          <t>MME213-2014-15-(11)</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(3)</t>
+          <t>MME235-2016-17-(1)</t>
         </is>
       </c>
     </row>
@@ -1441,17 +1441,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>MME235-2018-19-(8)</t>
+          <t>MME213-2018-19-(5)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(8)</t>
+          <t>MME213-2015-16-(10)</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(6)</t>
+          <t>MME235-2017-18-(7)</t>
         </is>
       </c>
     </row>
@@ -1461,17 +1461,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>EEE267-2014-15-(7)</t>
+          <t>ME221-2018-19-(6)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(4)</t>
+          <t>MME213-2014-15-(9)</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>MME235-2016-17-(1)</t>
+          <t>MME235-2018-19-(8)</t>
         </is>
       </c>
     </row>
@@ -1481,17 +1481,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>EEE267-2018-19-(7)</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>MME235-2015-16-(7)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>MME235-2015-16-(8)</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>MME213-2016-17-(6)</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>MME235-2018-19-(6)</t>
         </is>
       </c>
     </row>
@@ -1501,17 +1501,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>MME235-2014-15-(6)</t>
+          <t>ME221-2015-16-(4)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(1)</t>
+          <t>MME235-2015-16-(4)</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(3)</t>
+          <t>EEE267-2016-17-(6)</t>
         </is>
       </c>
     </row>
@@ -1521,17 +1521,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ME221-2014-15-(6)</t>
+          <t>MME213-2014-15-(4)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>EEE267-2018-19-(8)</t>
+          <t>EEE267-2018-19-(5)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>ME221-2018-19-(1)</t>
+          <t>EEE267-2018-19-(6)</t>
         </is>
       </c>
     </row>
@@ -1541,17 +1541,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ME221-2014-15-(8)</t>
+          <t>MME213-2017-18-(9)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(2)</t>
+          <t>MME213-2015-16-(3)</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>MME213-2017-18-(9)</t>
+          <t>EEE267-2016-17-(8)</t>
         </is>
       </c>
     </row>
@@ -1561,17 +1561,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>MME235-2017-18-(3)</t>
+          <t>ME221-2016-17-(6)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MME213-2014-15-(3)</t>
+          <t>EEE267-2017-18-(5)</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(5)</t>
+          <t>MME213-2017-18-(1)</t>
         </is>
       </c>
     </row>
@@ -1581,17 +1581,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>MME213-2018-19-(2)</t>
+          <t>ME221-2017-18-(1)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(2)</t>
+          <t>EEE267-2016-17-(1)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MME213-2017-18-(11)</t>
         </is>
       </c>
     </row>
@@ -1601,17 +1601,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>MME235-2018-19-(3)</t>
+          <t>MME235-2017-18-(1)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>EEE267-2015-16-(6)</t>
+          <t>ME221-2015-16-(3)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>MME213-2016-17-(1)</t>
+          <t>MME213-2016-17-(2)</t>
         </is>
       </c>
     </row>
@@ -1621,17 +1621,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>MME213-2015-16-(6)</t>
+          <t>MME213-2016-17-(4)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MME235-2018-19-(5)</t>
+          <t>MME213-2017-18-(6)</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(4)</t>
+          <t>ME221-2018-19-(5)</t>
         </is>
       </c>
     </row>
@@ -1641,17 +1641,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ME221-2016-17-(3)</t>
+          <t>ME221-2016-17-(4)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>EEE267-2017-18-(4)</t>
+          <t>MME235-2016-17-(6)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>EEE267-2016-17-(8)</t>
+          <t>EEE267-2015-16-(7)</t>
         </is>
       </c>
     </row>

</xml_diff>